<commit_message>
Recalibrate the model with obs till 2018-06-30 and update figures.
</commit_message>
<xml_diff>
--- a/data/default_starting_params.xlsx
+++ b/data/default_starting_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://anu365-my.sharepoint.com/personal/u1066632_anu_edu_au/Documents/WORKANU/Projects/GraphEvalUnc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{7C3EEB59-675A-4DCC-B94E-FFD84DC4581A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2483C108-A26B-46EB-B53E-090F167ED353}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{7C3EEB59-675A-4DCC-B94E-FFD84DC4581A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE9EF4E2-9240-463A-AFAC-4B40715D8C6A}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25005" yWindow="2205" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,12 +131,6 @@
     <t>ShortName</t>
   </si>
   <si>
-    <t>ScalingFactor (Subsurf)</t>
-  </si>
-  <si>
-    <t>ScalingFactor (Surf)</t>
-  </si>
-  <si>
     <t>EMC (Grazing)</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>DWC (Other)</t>
+  </si>
+  <si>
+    <t>ScaleFactor (Subsurf)</t>
+  </si>
+  <si>
+    <t>ScaleFactor (Surf)</t>
   </si>
 </sst>
 </file>
@@ -211,6 +211,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,7 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -547,7 +551,7 @@
         <v>0.5</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -576,7 +580,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -605,7 +609,7 @@
         <v>0.5</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -634,7 +638,7 @@
         <v>0.1</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -663,7 +667,7 @@
         <v>0.5</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -692,7 +696,7 @@
         <v>0.1</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -721,7 +725,7 @@
         <v>0.5</v>
       </c>
       <c r="I8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -750,7 +754,7 @@
         <v>0.1</v>
       </c>
       <c r="I9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -779,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -808,7 +812,7 @@
         <v>0.2</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>